<commit_message>
add for supplyment result analysis of alpha
</commit_message>
<xml_diff>
--- a/AddForSupplymentOfSMDHDPHMM/numofclusterVSalpha/result_analysis.xlsx
+++ b/AddForSupplymentOfSMDHDPHMM/numofclusterVSalpha/result_analysis.xlsx
@@ -14,13 +14,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>kxi</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始值类别个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聚类个数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -370,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="B2:D8"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1E-3</v>
       </c>
@@ -400,7 +412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -414,7 +426,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -428,7 +440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -442,7 +454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>10</v>
       </c>
@@ -456,7 +468,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>100</v>
       </c>
@@ -470,7 +482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -482,6 +494,120 @@
       </c>
       <c r="D8">
         <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>500</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>1000</v>
+      </c>
+      <c r="C17">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>1500</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2000</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>21</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2500</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>3000</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read input data in txt form
</commit_message>
<xml_diff>
--- a/AddForSupplymentOfSMDHDPHMM/numofclusterVSalpha/result_analysis.xlsx
+++ b/AddForSupplymentOfSMDHDPHMM/numofclusterVSalpha/result_analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>kxi</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聚类个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ebsilon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -382,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -610,6 +622,181 @@
         <v>18</v>
       </c>
     </row>
+    <row r="23" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>1E-3</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>0.01</v>
+      </c>
+      <c r="C27">
+        <v>31</v>
+      </c>
+      <c r="D27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>1000</v>
+      </c>
+      <c r="C32">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>39</v>
+      </c>
+      <c r="E32">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>1E-3</v>
+      </c>
+      <c r="C41">
+        <v>18</v>
+      </c>
+      <c r="D41">
+        <v>19</v>
+      </c>
+      <c r="E41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>0.01</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+      <c r="D42">
+        <v>19</v>
+      </c>
+      <c r="E42">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>0.1</v>
+      </c>
+      <c r="C43">
+        <v>18</v>
+      </c>
+      <c r="D43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>19</v>
+      </c>
+      <c r="D44">
+        <v>19</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>19</v>
+      </c>
+      <c r="D45">
+        <v>19</v>
+      </c>
+      <c r="E45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>100</v>
+      </c>
+      <c r="C46">
+        <v>21</v>
+      </c>
+      <c r="D46">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>